<commit_message>
Add code reference and ML recent project dataset
</commit_message>
<xml_diff>
--- a/simplesample.xlsx
+++ b/simplesample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\Documents\IFB-454 DEEP LEARNING\t2_dl_188\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A650BED-9073-4338-A953-E729E15D8025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6877E5C2-4011-421B-A1E7-04DC65C4D84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43F375F7-3DC9-4D6A-B222-8528D373B72A}"/>
   </bookViews>
@@ -43,8 +43,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,8 +80,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,302 +405,305 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="10.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
+      <c r="A2" s="1">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="D11">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
+      <c r="A14" s="1">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19">
-        <v>5</v>
-      </c>
-      <c r="C19">
-        <v>5</v>
-      </c>
-      <c r="D19">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <v>5</v>
-      </c>
-      <c r="D21">
+      <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>